<commit_message>
start specifying different infrastructure types (e.g., primary roads etc.)
</commit_message>
<xml_diff>
--- a/data/Vulnerability/Table_D3_Costs_V1.0.0.xlsx
+++ b/data/Vulnerability/Table_D3_Costs_V1.0.0.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773CEC69-6B67-40F2-8C7B-CD5A81A7FE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16391045-C532-4750-AE89-4653D562C16E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="2" r:id="rId1"/>
@@ -2040,14 +2040,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E197E81-434E-409D-932C-7BC6F31F433C}">
   <dimension ref="B1:AC53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:29" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:29" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
         <v>358</v>
       </c>
@@ -2067,7 +2067,7 @@
       <c r="P2" s="10"/>
       <c r="Q2" s="11"/>
     </row>
-    <row r="3" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -2085,7 +2085,7 @@
       <c r="P3" s="13"/>
       <c r="Q3" s="14"/>
     </row>
-    <row r="4" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -2103,7 +2103,7 @@
       <c r="P4" s="13"/>
       <c r="Q4" s="14"/>
     </row>
-    <row r="5" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
@@ -2121,7 +2121,7 @@
       <c r="P5" s="13"/>
       <c r="Q5" s="14"/>
     </row>
-    <row r="6" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B6" s="12"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -2139,7 +2139,7 @@
       <c r="P6" s="13"/>
       <c r="Q6" s="14"/>
     </row>
-    <row r="7" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B7" s="12"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -2157,7 +2157,7 @@
       <c r="P7" s="13"/>
       <c r="Q7" s="14"/>
     </row>
-    <row r="8" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -2175,7 +2175,7 @@
       <c r="P8" s="13"/>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -2193,7 +2193,7 @@
       <c r="P9" s="13"/>
       <c r="Q9" s="14"/>
     </row>
-    <row r="10" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -2211,7 +2211,7 @@
       <c r="P10" s="13"/>
       <c r="Q10" s="14"/>
     </row>
-    <row r="11" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -2229,7 +2229,7 @@
       <c r="P11" s="13"/>
       <c r="Q11" s="14"/>
     </row>
-    <row r="12" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -2257,7 +2257,7 @@
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
     </row>
-    <row r="13" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -2275,7 +2275,7 @@
       <c r="P13" s="13"/>
       <c r="Q13" s="14"/>
     </row>
-    <row r="14" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -2293,7 +2293,7 @@
       <c r="P14" s="13"/>
       <c r="Q14" s="14"/>
     </row>
-    <row r="15" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -2311,7 +2311,7 @@
       <c r="P15" s="13"/>
       <c r="Q15" s="14"/>
     </row>
-    <row r="16" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:29" x14ac:dyDescent="0.35">
       <c r="B16" s="12"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
@@ -2329,7 +2329,7 @@
       <c r="P16" s="13"/>
       <c r="Q16" s="14"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B17" s="12"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
@@ -2347,7 +2347,7 @@
       <c r="P17" s="13"/>
       <c r="Q17" s="14"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -2365,7 +2365,7 @@
       <c r="P18" s="13"/>
       <c r="Q18" s="14"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B19" s="12"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -2383,7 +2383,7 @@
       <c r="P19" s="13"/>
       <c r="Q19" s="14"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -2401,7 +2401,7 @@
       <c r="P20" s="13"/>
       <c r="Q20" s="14"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B21" s="12"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -2419,7 +2419,7 @@
       <c r="P21" s="13"/>
       <c r="Q21" s="14"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -2437,7 +2437,7 @@
       <c r="P22" s="13"/>
       <c r="Q22" s="14"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -2455,7 +2455,7 @@
       <c r="P23" s="13"/>
       <c r="Q23" s="14"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B24" s="12"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
@@ -2473,7 +2473,7 @@
       <c r="P24" s="13"/>
       <c r="Q24" s="14"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B25" s="12"/>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
@@ -2491,7 +2491,7 @@
       <c r="P25" s="13"/>
       <c r="Q25" s="14"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B26" s="12"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
@@ -2509,7 +2509,7 @@
       <c r="P26" s="13"/>
       <c r="Q26" s="14"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B27" s="12"/>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -2527,7 +2527,7 @@
       <c r="P27" s="13"/>
       <c r="Q27" s="14"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B28" s="12"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -2545,7 +2545,7 @@
       <c r="P28" s="13"/>
       <c r="Q28" s="14"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -2563,7 +2563,7 @@
       <c r="P29" s="13"/>
       <c r="Q29" s="14"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B30" s="12"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
@@ -2581,7 +2581,7 @@
       <c r="P30" s="13"/>
       <c r="Q30" s="14"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -2599,7 +2599,7 @@
       <c r="P31" s="13"/>
       <c r="Q31" s="14"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B32" s="12"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -2617,7 +2617,7 @@
       <c r="P32" s="13"/>
       <c r="Q32" s="14"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -2635,7 +2635,7 @@
       <c r="P33" s="13"/>
       <c r="Q33" s="14"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B34" s="12"/>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
@@ -2653,7 +2653,7 @@
       <c r="P34" s="13"/>
       <c r="Q34" s="14"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B35" s="12"/>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
@@ -2671,7 +2671,7 @@
       <c r="P35" s="13"/>
       <c r="Q35" s="14"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B36" s="12"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
@@ -2689,7 +2689,7 @@
       <c r="P36" s="13"/>
       <c r="Q36" s="14"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B37" s="12"/>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
@@ -2707,7 +2707,7 @@
       <c r="P37" s="13"/>
       <c r="Q37" s="14"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B38" s="12"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
@@ -2725,7 +2725,7 @@
       <c r="P38" s="13"/>
       <c r="Q38" s="14"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B39" s="12"/>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
@@ -2743,7 +2743,7 @@
       <c r="P39" s="13"/>
       <c r="Q39" s="14"/>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B40" s="12"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
@@ -2761,7 +2761,7 @@
       <c r="P40" s="13"/>
       <c r="Q40" s="14"/>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B41" s="12"/>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
@@ -2779,7 +2779,7 @@
       <c r="P41" s="13"/>
       <c r="Q41" s="14"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B42" s="12"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
@@ -2797,7 +2797,7 @@
       <c r="P42" s="13"/>
       <c r="Q42" s="14"/>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B43" s="12"/>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
@@ -2815,7 +2815,7 @@
       <c r="P43" s="13"/>
       <c r="Q43" s="14"/>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B44" s="12"/>
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
@@ -2833,7 +2833,7 @@
       <c r="P44" s="13"/>
       <c r="Q44" s="14"/>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B45" s="12"/>
       <c r="C45" s="13"/>
       <c r="D45" s="13"/>
@@ -2851,7 +2851,7 @@
       <c r="P45" s="13"/>
       <c r="Q45" s="14"/>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B46" s="12"/>
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
@@ -2869,7 +2869,7 @@
       <c r="P46" s="13"/>
       <c r="Q46" s="14"/>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B47" s="12"/>
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
@@ -2887,7 +2887,7 @@
       <c r="P47" s="13"/>
       <c r="Q47" s="14"/>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B48" s="12"/>
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
@@ -2905,7 +2905,7 @@
       <c r="P48" s="13"/>
       <c r="Q48" s="14"/>
     </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B49" s="12"/>
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
@@ -2923,7 +2923,7 @@
       <c r="P49" s="13"/>
       <c r="Q49" s="14"/>
     </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B50" s="12"/>
       <c r="C50" s="13"/>
       <c r="D50" s="13"/>
@@ -2941,7 +2941,7 @@
       <c r="P50" s="13"/>
       <c r="Q50" s="14"/>
     </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B51" s="12"/>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
@@ -2959,7 +2959,7 @@
       <c r="P51" s="13"/>
       <c r="Q51" s="14"/>
     </row>
-    <row r="52" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B52" s="15"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -2977,7 +2977,7 @@
       <c r="P52" s="16"/>
       <c r="Q52" s="17"/>
     </row>
-    <row r="53" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="2:17" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:Q52"/>
@@ -2991,28 +2991,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF54DA9-9DBA-41E5-8892-C2F99E6F867D}">
   <dimension ref="A1:J180"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.54296875" customWidth="1"/>
+    <col min="2" max="2" width="42.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="78.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="72.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="78.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="72.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>92</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>100</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>119</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>107</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>188</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>105</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>109</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>181</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>181</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>181</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>181</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>103</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>177</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>177</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>177</v>
       </c>
@@ -3867,7 +3867,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>177</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>174</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>174</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>174</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>175</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>175</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>179</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>179</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>179</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>179</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>180</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>96</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>96</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>96</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>155</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>80</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>80</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
         <v>70</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>70</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>70</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>70</v>
       </c>
@@ -4690,7 +4690,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
         <v>70</v>
       </c>
@@ -4882,7 +4882,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="6" t="s">
         <v>70</v>
       </c>
@@ -4914,7 +4914,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
         <v>70</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -5010,7 +5010,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>42</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>42</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>42</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>42</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>42</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>42</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>42</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>42</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>42</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>42</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>42</v>
       </c>
@@ -5362,7 +5362,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>42</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>42</v>
       </c>
@@ -5426,7 +5426,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>42</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>42</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>42</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>42</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>42</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>42</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>42</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>42</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>42</v>
       </c>
@@ -5714,7 +5714,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>42</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>42</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>42</v>
       </c>
@@ -5810,7 +5810,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>42</v>
       </c>
@@ -5842,7 +5842,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>42</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>42</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>111</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>111</v>
       </c>
@@ -5970,7 +5970,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>41</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>19</v>
       </c>
@@ -6034,7 +6034,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>19</v>
       </c>
@@ -6066,7 +6066,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>19</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>19</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="6" t="s">
         <v>256</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>280</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>280</v>
       </c>
@@ -6226,7 +6226,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>178</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -6319,7 +6319,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>94</v>
       </c>
@@ -6351,7 +6351,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>94</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>94</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>94</v>
       </c>
@@ -6447,7 +6447,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>94</v>
       </c>
@@ -6479,7 +6479,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>95</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>95</v>
       </c>
@@ -6543,7 +6543,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>95</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>176</v>
       </c>
@@ -6607,7 +6607,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>13</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>13</v>
       </c>
@@ -6671,7 +6671,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>13</v>
       </c>
@@ -6703,7 +6703,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>13</v>
       </c>
@@ -6735,7 +6735,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>13</v>
       </c>
@@ -6767,7 +6767,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>13</v>
       </c>
@@ -6799,7 +6799,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>13</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>13</v>
       </c>
@@ -6863,7 +6863,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>13</v>
       </c>
@@ -6895,7 +6895,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>13</v>
       </c>
@@ -6927,7 +6927,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>13</v>
       </c>
@@ -6959,7 +6959,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>13</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>13</v>
       </c>
@@ -7023,7 +7023,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>13</v>
       </c>
@@ -7055,7 +7055,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>13</v>
       </c>
@@ -7087,7 +7087,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>13</v>
       </c>
@@ -7119,7 +7119,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>13</v>
       </c>
@@ -7151,7 +7151,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>13</v>
       </c>
@@ -7183,7 +7183,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>13</v>
       </c>
@@ -7215,7 +7215,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>13</v>
       </c>
@@ -7247,7 +7247,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>13</v>
       </c>
@@ -7279,7 +7279,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>13</v>
       </c>
@@ -7311,7 +7311,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>13</v>
       </c>
@@ -7343,7 +7343,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>13</v>
       </c>
@@ -7375,7 +7375,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>13</v>
       </c>
@@ -7407,7 +7407,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>13</v>
       </c>
@@ -7439,7 +7439,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>13</v>
       </c>
@@ -7471,7 +7471,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>13</v>
       </c>
@@ -7503,7 +7503,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>13</v>
       </c>
@@ -7535,7 +7535,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>13</v>
       </c>
@@ -7567,7 +7567,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>13</v>
       </c>
@@ -7599,7 +7599,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>13</v>
       </c>
@@ -7631,7 +7631,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>13</v>
       </c>
@@ -7663,7 +7663,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>13</v>
       </c>
@@ -7695,7 +7695,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>13</v>
       </c>
@@ -7727,7 +7727,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>13</v>
       </c>
@@ -7759,7 +7759,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>13</v>
       </c>
@@ -7791,7 +7791,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>13</v>
       </c>
@@ -7823,7 +7823,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>13</v>
       </c>
@@ -7855,7 +7855,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>13</v>
       </c>
@@ -7887,7 +7887,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>13</v>
       </c>
@@ -7919,7 +7919,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>13</v>
       </c>
@@ -7951,7 +7951,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>13</v>
       </c>
@@ -7983,7 +7983,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>13</v>
       </c>
@@ -8015,7 +8015,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>13</v>
       </c>
@@ -8047,7 +8047,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>13</v>
       </c>
@@ -8079,7 +8079,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>13</v>
       </c>
@@ -8111,7 +8111,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>13</v>
       </c>
@@ -8143,7 +8143,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>13</v>
       </c>
@@ -8175,7 +8175,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>13</v>
       </c>
@@ -8207,7 +8207,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>13</v>
       </c>
@@ -8239,7 +8239,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>13</v>
       </c>
@@ -8271,7 +8271,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>13</v>
       </c>
@@ -8303,7 +8303,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>13</v>
       </c>
@@ -8335,7 +8335,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>13</v>
       </c>
@@ -8367,7 +8367,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>13</v>
       </c>
@@ -8399,7 +8399,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>13</v>
       </c>
@@ -8431,7 +8431,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>13</v>
       </c>
@@ -8463,7 +8463,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>13</v>
       </c>
@@ -8495,7 +8495,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>13</v>
       </c>
@@ -8527,7 +8527,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>13</v>
       </c>
@@ -8559,7 +8559,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>13</v>
       </c>
@@ -8591,7 +8591,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>13</v>
       </c>
@@ -8623,7 +8623,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>13</v>
       </c>
@@ -8655,7 +8655,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>13</v>
       </c>
@@ -8687,7 +8687,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>13</v>
       </c>
@@ -8719,7 +8719,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>13</v>
       </c>
@@ -8770,119 +8770,119 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>243</v>
       </c>

</xml_diff>